<commit_message>
Increased baud rate from teensy4.1 to WizFi360 from 1M to 1.5M
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacly\Documents\WDA\WDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E497536-FEDE-4EF9-9EA2-00B1CD9B1735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB6ADF3-4DF7-4C77-94A3-F4A6D6C116F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{EAE9CD10-43FF-4944-B7EF-D58447343E10}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Testing" sheetId="1" r:id="rId1"/>
     <sheet name="Improvement Plan" sheetId="2" r:id="rId2"/>
+    <sheet name="Reporting Speed" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>Test Time</t>
   </si>
@@ -215,6 +216,78 @@
   </si>
   <si>
     <t>threads? Multiprocessing? Better understanding of the plotting functions?</t>
+  </si>
+  <si>
+    <t>(2 System, 1 Ch) - Make all tests end with the correct number of smaples</t>
+  </si>
+  <si>
+    <t>PC Side - Separate the check for "END" by device</t>
+  </si>
+  <si>
+    <t>GOOD</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>on_message()</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Channels</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Actual Time - Initial</t>
+  </si>
+  <si>
+    <t>Actual Time - Final</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>1.5M</t>
+  </si>
+  <si>
+    <t>WizFi Baud</t>
+  </si>
+  <si>
+    <t>The bottleneck in terms of reporting speed is the how fast the Teensy and WizFi can send data. The slowest part in this chain is the serial communication from Teensy to WizFi</t>
+  </si>
+  <si>
+    <t>So, in order to improve performance, the baud rate for that serial connection was increased from 1M to 1.5M. WizFi360 max baud rate is 2M.</t>
+  </si>
+  <si>
+    <t>1.1 - Fix</t>
+  </si>
+  <si>
+    <t>Sometimes more samples than expected are received</t>
+  </si>
+  <si>
+    <t>Sometimes when using 2 sensors, less samples than expected are received</t>
+  </si>
+  <si>
+    <t>2.1 - Fix</t>
+  </si>
+  <si>
+    <t>It takes longer to report the data than it does to record it</t>
+  </si>
+  <si>
+    <t>3.1 - Fix</t>
+  </si>
+  <si>
+    <t>Increased baud rate from 1M to 1.5M</t>
   </si>
 </sst>
 </file>
@@ -272,7 +345,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -691,62 +764,12 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -807,11 +830,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -852,37 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -904,34 +912,61 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -946,88 +981,193 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1036,20 +1176,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,6 +1227,996 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Reporting Speed'!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Time - Initial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Reporting Speed'!$E$5:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Reporting Speed'!$F$5:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D2FA-4F3D-96D0-92ACC6985CD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Reporting Speed'!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Time - Final</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Reporting Speed'!$E$5:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Reporting Speed'!$G$5:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D2FA-4F3D-96D0-92ACC6985CD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="770143712"/>
+        <c:axId val="864783328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="770143712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="864783328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="864783328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="770143712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>54768</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>602455</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DFFF7C4-E4DE-F0A2-72D4-F3BD24101312}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1385,22 +2531,22 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="20"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="36"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B3" s="7" t="s">
@@ -1445,10 +2591,10 @@
       <c r="C4" s="2">
         <v>1000</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="15">
         <v>5000</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="20">
         <v>5</v>
       </c>
       <c r="G4" s="6">
@@ -1461,16 +2607,16 @@
       <c r="J4" s="3">
         <v>1000</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="15">
         <v>5000</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="16">
         <v>5000</v>
       </c>
-      <c r="M4" s="26">
+      <c r="M4" s="16">
         <v>5000</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="19">
         <v>13</v>
       </c>
     </row>
@@ -1484,7 +2630,7 @@
       <c r="D5" s="11">
         <v>6002</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="20">
         <v>5</v>
       </c>
       <c r="G5" s="6">
@@ -1506,7 +2652,7 @@
       <c r="M5" s="12">
         <v>6002</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="21">
         <v>5</v>
       </c>
     </row>
@@ -1520,7 +2666,7 @@
       <c r="D6" s="11">
         <v>7507</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="20">
         <v>5</v>
       </c>
       <c r="G6" s="6">
@@ -1553,10 +2699,10 @@
       <c r="C7" s="2">
         <v>2000</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="15">
         <v>10000</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="20">
         <v>5</v>
       </c>
       <c r="G7" s="6">
@@ -1569,16 +2715,16 @@
       <c r="J7" s="3">
         <v>2000</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="15">
         <v>10000</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="16">
         <v>10000</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M7" s="16">
         <v>10000</v>
       </c>
-      <c r="N7" s="29">
+      <c r="N7" s="19">
         <v>11</v>
       </c>
     </row>
@@ -1589,10 +2735,10 @@
       <c r="C8" s="2">
         <v>1000</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="15">
         <v>10000</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="20">
         <v>10</v>
       </c>
       <c r="G8" s="6">
@@ -1605,16 +2751,16 @@
       <c r="J8" s="3">
         <v>1000</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="15">
         <v>10000</v>
       </c>
-      <c r="L8" s="26">
+      <c r="L8" s="16">
         <v>10000</v>
       </c>
-      <c r="M8" s="26">
+      <c r="M8" s="16">
         <v>10000</v>
       </c>
-      <c r="N8" s="29">
+      <c r="N8" s="19">
         <v>40</v>
       </c>
     </row>
@@ -1628,7 +2774,7 @@
       <c r="D9" s="11">
         <v>12004</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="20">
         <v>10</v>
       </c>
       <c r="G9" s="6">
@@ -1664,7 +2810,7 @@
       <c r="D10" s="11">
         <v>15015</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="20">
         <v>11</v>
       </c>
       <c r="G10" s="6">
@@ -1686,7 +2832,7 @@
       <c r="M10" s="12">
         <v>15015</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10" s="19">
         <v>21</v>
       </c>
     </row>
@@ -1697,10 +2843,10 @@
       <c r="C11" s="2">
         <v>2000</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="15">
         <v>20000</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="20">
         <v>10</v>
       </c>
       <c r="G11" s="6">
@@ -1713,40 +2859,40 @@
       <c r="J11" s="3">
         <v>2000</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="15">
         <v>20000</v>
       </c>
-      <c r="L11" s="26">
+      <c r="L11" s="16">
         <v>20000</v>
       </c>
-      <c r="M11" s="26">
+      <c r="M11" s="16">
         <v>20000</v>
       </c>
-      <c r="N11" s="29">
+      <c r="N11" s="19">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="20" spans="2:17" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="I20" s="17" t="s">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="14"/>
+      <c r="I20" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="21"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="37"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21" s="7" t="s">
@@ -1764,7 +2910,7 @@
       <c r="F21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="23"/>
+      <c r="G21" s="5"/>
       <c r="I21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1800,38 +2946,38 @@
       <c r="C22" s="3">
         <v>1000</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="15">
         <v>5000</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="16">
         <v>5000</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="19">
         <v>30</v>
       </c>
-      <c r="G22" s="24"/>
+      <c r="G22" s="6"/>
       <c r="I22" s="1">
         <v>5</v>
       </c>
       <c r="J22" s="3">
         <v>1000</v>
       </c>
-      <c r="K22" s="27">
+      <c r="K22" s="17">
         <v>4953</v>
       </c>
-      <c r="L22" s="27">
+      <c r="L22" s="17">
         <v>4953</v>
       </c>
-      <c r="M22" s="27">
+      <c r="M22" s="17">
         <v>4953</v>
       </c>
-      <c r="N22" s="27">
+      <c r="N22" s="17">
         <v>4953</v>
       </c>
-      <c r="O22" s="27">
+      <c r="O22" s="17">
         <v>4953</v>
       </c>
-      <c r="P22" s="27">
+      <c r="P22" s="17">
         <v>4953</v>
       </c>
       <c r="Q22" s="2">
@@ -1845,38 +2991,38 @@
       <c r="C23" s="3">
         <v>1200</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="17">
         <v>5706</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="18">
         <v>5706</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="19">
         <v>30</v>
       </c>
-      <c r="G23" s="24"/>
+      <c r="G23" s="6"/>
       <c r="I23" s="1">
         <v>5</v>
       </c>
       <c r="J23" s="3">
         <v>1200</v>
       </c>
-      <c r="K23" s="27">
+      <c r="K23" s="17">
         <v>5771</v>
       </c>
-      <c r="L23" s="27">
+      <c r="L23" s="17">
         <v>5771</v>
       </c>
-      <c r="M23" s="27">
+      <c r="M23" s="17">
         <v>5771</v>
       </c>
-      <c r="N23" s="27">
+      <c r="N23" s="17">
         <v>5771</v>
       </c>
-      <c r="O23" s="27">
+      <c r="O23" s="17">
         <v>5771</v>
       </c>
-      <c r="P23" s="27">
+      <c r="P23" s="17">
         <v>5771</v>
       </c>
       <c r="Q23" s="2">
@@ -1896,10 +3042,10 @@
       <c r="E24" s="12">
         <v>7506</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="19">
         <v>35</v>
       </c>
-      <c r="G24" s="24"/>
+      <c r="G24" s="6"/>
       <c r="I24" s="1">
         <v>5</v>
       </c>
@@ -1935,38 +3081,38 @@
       <c r="C25" s="3">
         <v>2000</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="17">
         <v>9716</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25" s="18">
         <v>9716</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="19">
         <v>35</v>
       </c>
-      <c r="G25" s="24"/>
+      <c r="G25" s="6"/>
       <c r="I25" s="1">
         <v>5</v>
       </c>
       <c r="J25" s="3">
         <v>2000</v>
       </c>
-      <c r="K25" s="27">
+      <c r="K25" s="17">
         <v>9258</v>
       </c>
-      <c r="L25" s="27">
+      <c r="L25" s="17">
         <v>9258</v>
       </c>
-      <c r="M25" s="27">
+      <c r="M25" s="17">
         <v>9258</v>
       </c>
-      <c r="N25" s="27">
+      <c r="N25" s="17">
         <v>9258</v>
       </c>
-      <c r="O25" s="27">
+      <c r="O25" s="17">
         <v>9258</v>
       </c>
-      <c r="P25" s="27">
+      <c r="P25" s="17">
         <v>9258</v>
       </c>
       <c r="Q25" s="2">
@@ -1980,16 +3126,16 @@
       <c r="C26" s="3">
         <v>1000</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="17">
         <v>9825</v>
       </c>
-      <c r="E26" s="28">
+      <c r="E26" s="18">
         <v>9825</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="19">
         <v>46</v>
       </c>
-      <c r="G26" s="24"/>
+      <c r="G26" s="6"/>
       <c r="I26" s="1">
         <v>10</v>
       </c>
@@ -2019,10 +3165,10 @@
       <c r="E27" s="12">
         <v>12004</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="19">
         <v>63</v>
       </c>
-      <c r="G27" s="24"/>
+      <c r="G27" s="6"/>
       <c r="I27" s="1">
         <v>10</v>
       </c>
@@ -2050,10 +3196,10 @@
       <c r="E28" s="12">
         <v>15015</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="19">
         <v>51</v>
       </c>
-      <c r="G28" s="24"/>
+      <c r="G28" s="6"/>
       <c r="I28" s="1">
         <v>10</v>
       </c>
@@ -2075,16 +3221,16 @@
       <c r="C29" s="3">
         <v>2000</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="17">
         <v>19450</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="18">
         <v>19450</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="19">
         <v>48</v>
       </c>
-      <c r="G29" s="24"/>
+      <c r="G29" s="6"/>
       <c r="I29" s="1">
         <v>10</v>
       </c>
@@ -2100,16 +3246,16 @@
       <c r="Q29" s="2"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="G30" s="24"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="G31" s="24"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="G32" s="24"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.45">
-      <c r="G33" s="24"/>
+      <c r="G33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2125,309 +3271,605 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A786F96C-C7B4-4D87-9393-B94FC3ACB139}">
-  <dimension ref="B1:Q20"/>
+  <dimension ref="B1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="70" t="s">
+    <row r="1" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="72"/>
-    </row>
-    <row r="3" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="39">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52"/>
+    </row>
+    <row r="3" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="53">
         <v>1</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="75"/>
-      <c r="K3" s="42" t="s">
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="59"/>
+      <c r="K3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="44"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B4" s="40"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="53"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="47"/>
-    </row>
-    <row r="5" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="41">
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="43"/>
+      <c r="S3" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B4" s="54"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
+      <c r="S4" s="28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B5" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="104" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="103"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="46"/>
+      <c r="S5" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="69"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="47"/>
-    </row>
-    <row r="6" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="K6" s="48"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="50"/>
-    </row>
-    <row r="7" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B8" s="63">
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="49"/>
+    </row>
+    <row r="7" spans="2:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+      <c r="N7" s="101"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+    </row>
+    <row r="8" spans="2:19" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="101"/>
+      <c r="Q8" s="101"/>
+    </row>
+    <row r="9" spans="2:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="63">
         <v>2</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C9" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+    </row>
+    <row r="10" spans="2:19" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="64"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+    </row>
+    <row r="11" spans="2:19" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="26">
+        <v>2.1</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+    </row>
+    <row r="12" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="73"/>
+    </row>
+    <row r="13" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B14" s="55">
+        <v>3</v>
+      </c>
+      <c r="C14" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="44"/>
-    </row>
-    <row r="9" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="65"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
-    </row>
-    <row r="10" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="63">
-        <v>2.1</v>
-      </c>
-      <c r="C10" s="60" t="s">
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
+    </row>
+    <row r="15" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="56"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
+    </row>
+    <row r="16" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="105">
+        <v>3.1</v>
+      </c>
+      <c r="C16" s="107" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="108"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="108"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="109"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B17" s="74"/>
+      <c r="C17" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="62"/>
-      <c r="K10" s="42" t="s">
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="106"/>
+      <c r="I17" s="111"/>
+      <c r="K17" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="33"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B11" s="64"/>
-      <c r="C11" s="57" t="s">
+      <c r="L17" s="75"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="76"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B18" s="74"/>
+      <c r="C18" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58" t="s">
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="36"/>
-    </row>
-    <row r="12" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="64"/>
-      <c r="C12" s="52" t="s">
+      <c r="G18" s="102"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="103"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="77"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="77"/>
+      <c r="O18" s="77"/>
+      <c r="P18" s="77"/>
+      <c r="Q18" s="78"/>
+    </row>
+    <row r="19" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="74"/>
+      <c r="C19" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51" t="s">
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="53"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="36"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B13" s="64"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="53"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="36"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B14" s="64"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="53"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="36"/>
-    </row>
-    <row r="15" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="65"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="56"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="38"/>
-    </row>
-    <row r="17" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="18" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="63">
-        <v>3</v>
-      </c>
-      <c r="C18" s="42" t="s">
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="62"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="77"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="77"/>
+      <c r="Q19" s="78"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B20" s="74"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="77"/>
+      <c r="Q20" s="78"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B21" s="74"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="62"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="77"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="77"/>
+      <c r="P21" s="77"/>
+      <c r="Q21" s="78"/>
+    </row>
+    <row r="22" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="79"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="90"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="81"/>
+    </row>
+    <row r="23" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B23" s="112" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="113" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="114"/>
+    </row>
+    <row r="26" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="27" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="55">
+        <v>4</v>
+      </c>
+      <c r="C27" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="44"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B19" s="80"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="79"/>
-    </row>
-    <row r="20" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="41">
-        <v>3.1</v>
-      </c>
-      <c r="C20" s="67" t="s">
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="43"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B28" s="82"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="85"/>
+    </row>
+    <row r="29" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C29" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="69"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="88"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="K10:Q15"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:I19"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C12:E15"/>
-    <mergeCell ref="F12:I15"/>
-    <mergeCell ref="C10:I10"/>
+  <mergeCells count="25">
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C19:E22"/>
+    <mergeCell ref="F19:I22"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="K3:Q6"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:I18"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="C3:I4"/>
-    <mergeCell ref="C8:I9"/>
+    <mergeCell ref="C14:I15"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:I10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K17:Q22"/>
+    <mergeCell ref="C17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3759C2C1-CE5A-49BD-842C-778D21E6A6E0}">
+  <dimension ref="B1:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="6" width="16.46484375" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B3" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="J3" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="94"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="95"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="97"/>
+    </row>
+    <row r="5" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>11</v>
+      </c>
+      <c r="J5" s="98"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="99"/>
+      <c r="N5" s="100"/>
+    </row>
+    <row r="6" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>35</v>
+      </c>
+      <c r="G6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>32</v>
+      </c>
+      <c r="J7" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="94"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J8" s="95"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
+    </row>
+    <row r="9" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="J9" s="98"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="100"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="J3:N5"/>
+    <mergeCell ref="J7:N9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>